<commit_message>
Add report and chart of papertrade
</commit_message>
<xml_diff>
--- a/assignment1/report.xlsx
+++ b/assignment1/report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>EQUITY</t>
   </si>
@@ -31,15 +31,26 @@
   </si>
   <si>
     <t># Shares</t>
+  </si>
+  <si>
+    <t>EP</t>
+  </si>
+  <si>
+    <t>ISRG</t>
+  </si>
+  <si>
+    <t>CMD</t>
+  </si>
+  <si>
+    <t>OKE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -78,9 +89,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -386,7 +398,7 @@
   <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,42 +430,63 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>13.72</v>
       </c>
       <c r="D4">
         <v>0.1</v>
       </c>
-      <c r="E4" s="1">
-        <f>C2*D4/C4</f>
-        <v>100000</v>
+      <c r="E4" s="2">
+        <f>$C$2*D4/C4</f>
+        <v>7288.6297376093289</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>269</v>
+      </c>
       <c r="D5">
         <v>0.1</v>
       </c>
-      <c r="E5" s="1" t="e">
-        <f t="shared" ref="E5:E7" si="0">C3*D5/C5</f>
-        <v>#VALUE!</v>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E7" si="0">$C$2*D5/C5</f>
+        <v>371.74721189591077</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>47.55</v>
+      </c>
       <c r="D6">
-        <v>0.1</v>
-      </c>
-      <c r="E6" s="1" t="e">
+        <v>0.3</v>
+      </c>
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>6309.1482649842274</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>26.76</v>
+      </c>
       <c r="D7">
-        <v>0.1</v>
-      </c>
-      <c r="E7" s="1" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>18684.603886397606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>